<commit_message>
excel file added for data
</commit_message>
<xml_diff>
--- a/src/test/java/netBankingTestData/testData.xlsx
+++ b/src/test/java/netBankingTestData/testData.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16260" windowHeight="3375"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="testData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -399,10 +398,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -438,10 +440,10 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maven surefire plugin added to pom
</commit_message>
<xml_diff>
--- a/src/test/java/netBankingTestData/testData.xlsx
+++ b/src/test/java/netBankingTestData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>qapydAq</t>
   </si>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -416,33 +416,25 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>